<commit_message>
makes small code changes to emission scaling functions, updates UNFCCC mapping
</commit_message>
<xml_diff>
--- a/input/mappings/scaling/UNFCCC_scaling_mapping.xlsx
+++ b/input/mappings/scaling/UNFCCC_scaling_mapping.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26221"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="8620" yWindow="2260" windowWidth="12680" windowHeight="14920" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14300" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="map" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="140">
   <si>
     <t>description</t>
   </si>
@@ -44,9 +44,6 @@
     <t>industry</t>
   </si>
   <si>
-    <t>constant</t>
-  </si>
-  <si>
     <t>1.A</t>
   </si>
   <si>
@@ -68,9 +65,6 @@
     <t>domestic_transport</t>
   </si>
   <si>
-    <t>linear</t>
-  </si>
-  <si>
     <t>1.A.4</t>
   </si>
   <si>
@@ -440,20 +434,20 @@
     <t>ceds_sector</t>
   </si>
   <si>
-    <t>all</t>
-  </si>
-  <si>
     <t>pre_ext_year</t>
   </si>
   <si>
     <t>post_ext_year</t>
+  </si>
+  <si>
+    <t>NA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -477,13 +471,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -502,7 +489,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="29">
+  <cellStyleXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -532,12 +519,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="29">
+  <cellStyles count="31">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -552,6 +540,7 @@
     <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -566,6 +555,7 @@
     <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -897,7 +887,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D69"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -905,16 +895,16 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -958,160 +948,160 @@
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
         <v>8</v>
-      </c>
-      <c r="B8" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" t="s">
         <v>10</v>
-      </c>
-      <c r="B9" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" t="s">
         <v>12</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>13</v>
-      </c>
-      <c r="C10" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" t="s">
         <v>16</v>
       </c>
-      <c r="B11" t="s">
+      <c r="D11" t="s">
         <v>17</v>
-      </c>
-      <c r="C11" t="s">
-        <v>18</v>
-      </c>
-      <c r="D11" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12" t="s">
         <v>20</v>
-      </c>
-      <c r="B12" t="s">
-        <v>21</v>
-      </c>
-      <c r="C12" t="s">
-        <v>18</v>
-      </c>
-      <c r="D12" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" t="s">
+        <v>16</v>
+      </c>
+      <c r="D13" t="s">
         <v>23</v>
-      </c>
-      <c r="B13" t="s">
-        <v>24</v>
-      </c>
-      <c r="C13" t="s">
-        <v>18</v>
-      </c>
-      <c r="D13" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B14" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C14" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" t="s">
+        <v>16</v>
+      </c>
+      <c r="D15" t="s">
         <v>28</v>
-      </c>
-      <c r="B15" t="s">
-        <v>29</v>
-      </c>
-      <c r="C15" t="s">
-        <v>18</v>
-      </c>
-      <c r="D15" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B16" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C16" t="s">
         <v>6</v>
       </c>
       <c r="D16" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B17" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C17" t="s">
         <v>6</v>
       </c>
       <c r="D17" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B18" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C18" t="s">
         <v>6</v>
       </c>
       <c r="D18" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B19" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C19" t="s">
         <v>6</v>
       </c>
       <c r="D19" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B20" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C20" t="s">
         <v>6</v>
@@ -1119,10 +1109,10 @@
     </row>
     <row r="21" spans="1:4">
       <c r="A21" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B21" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C21" t="s">
         <v>6</v>
@@ -1130,91 +1120,91 @@
     </row>
     <row r="22" spans="1:4">
       <c r="A22" t="s">
+        <v>44</v>
+      </c>
+      <c r="B22" t="s">
+        <v>45</v>
+      </c>
+      <c r="C22" t="s">
+        <v>13</v>
+      </c>
+      <c r="D22" t="s">
         <v>46</v>
-      </c>
-      <c r="B22" t="s">
-        <v>47</v>
-      </c>
-      <c r="C22" t="s">
-        <v>14</v>
-      </c>
-      <c r="D22" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" t="s">
+        <v>47</v>
+      </c>
+      <c r="B23" t="s">
+        <v>48</v>
+      </c>
+      <c r="C23" t="s">
+        <v>13</v>
+      </c>
+      <c r="D23" t="s">
         <v>49</v>
-      </c>
-      <c r="B23" t="s">
-        <v>50</v>
-      </c>
-      <c r="C23" t="s">
-        <v>14</v>
-      </c>
-      <c r="D23" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" t="s">
+        <v>50</v>
+      </c>
+      <c r="B24" t="s">
+        <v>51</v>
+      </c>
+      <c r="C24" t="s">
+        <v>13</v>
+      </c>
+      <c r="D24" t="s">
         <v>52</v>
-      </c>
-      <c r="B24" t="s">
-        <v>53</v>
-      </c>
-      <c r="C24" t="s">
-        <v>14</v>
-      </c>
-      <c r="D24" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" t="s">
+        <v>53</v>
+      </c>
+      <c r="B25" t="s">
+        <v>54</v>
+      </c>
+      <c r="C25" t="s">
+        <v>13</v>
+      </c>
+      <c r="D25" t="s">
         <v>55</v>
-      </c>
-      <c r="B25" t="s">
-        <v>56</v>
-      </c>
-      <c r="C25" t="s">
-        <v>14</v>
-      </c>
-      <c r="D25" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="26" spans="1:4">
       <c r="A26" t="s">
+        <v>56</v>
+      </c>
+      <c r="B26" t="s">
+        <v>57</v>
+      </c>
+      <c r="C26" t="s">
         <v>58</v>
       </c>
-      <c r="B26" t="s">
+      <c r="D26" t="s">
         <v>59</v>
-      </c>
-      <c r="C26" t="s">
-        <v>60</v>
-      </c>
-      <c r="D26" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="27" spans="1:4">
       <c r="A27" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B27" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C27" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="28" spans="1:4">
       <c r="A28" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B28" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C28" t="s">
         <v>6</v>
@@ -1222,10 +1212,10 @@
     </row>
     <row r="29" spans="1:4">
       <c r="A29" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B29" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C29" t="s">
         <v>6</v>
@@ -1233,282 +1223,282 @@
     </row>
     <row r="30" spans="1:4">
       <c r="A30" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B30" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C30" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="31" spans="1:4">
       <c r="A31" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B31" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B32" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B33" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="34" spans="1:2">
       <c r="A34" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B34" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="35" spans="1:2">
       <c r="A35" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B35" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="36" spans="1:2">
       <c r="A36" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B36" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="37" spans="1:2">
       <c r="A37" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B37" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="38" spans="1:2">
       <c r="A38" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B38" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="39" spans="1:2">
       <c r="A39" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B39" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="40" spans="1:2">
       <c r="A40" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B40" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="41" spans="1:2">
       <c r="A41" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B41" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="42" spans="1:2">
       <c r="A42" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B42" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="43" spans="1:2">
       <c r="A43" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B43" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="44" spans="1:2">
       <c r="A44" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B44" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="45" spans="1:2">
       <c r="A45" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B45" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="46" spans="1:2">
       <c r="A46" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B46" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="47" spans="1:2">
       <c r="A47" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B47" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="48" spans="1:2">
       <c r="A48" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B48" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="49" spans="1:4">
       <c r="A49" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B49" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="50" spans="1:4">
       <c r="A50" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B50" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="51" spans="1:4">
       <c r="A51" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B51" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="52" spans="1:4">
       <c r="A52" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B52" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="53" spans="1:4">
       <c r="A53" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B53" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="54" spans="1:4">
       <c r="A54" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B54" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="55" spans="1:4">
       <c r="A55" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B55" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="56" spans="1:4">
       <c r="A56" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B56" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="57" spans="1:4">
       <c r="A57" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B57" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="58" spans="1:4">
       <c r="A58" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B58" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="59" spans="1:4">
       <c r="A59" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C59" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D59" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="60" spans="1:4">
       <c r="A60" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="61" spans="1:4">
       <c r="A61" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C61" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D61" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="62" spans="1:4">
       <c r="A62" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="63" spans="1:4">
       <c r="A63" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="64" spans="1:4">
       <c r="C64" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D64" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="65" spans="3:4">
@@ -1516,7 +1506,7 @@
         <v>6</v>
       </c>
       <c r="D65" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="66" spans="3:4">
@@ -1524,7 +1514,7 @@
         <v>6</v>
       </c>
       <c r="D66" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="67" spans="3:4">
@@ -1532,7 +1522,7 @@
         <v>6</v>
       </c>
       <c r="D67" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="68" spans="3:4">
@@ -1540,7 +1530,7 @@
         <v>6</v>
       </c>
       <c r="D68" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="69" spans="3:4">
@@ -1548,7 +1538,7 @@
         <v>6</v>
       </c>
       <c r="D69" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
   </sheetData>
@@ -1564,10 +1554,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1579,10 +1569,10 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B1" t="s">
         <v>135</v>
-      </c>
-      <c r="B1" t="s">
-        <v>137</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -1598,68 +1588,17 @@
       <c r="A2" t="s">
         <v>139</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>18</v>
+      <c r="B2" t="s">
+        <v>139</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>139</v>
       </c>
       <c r="D2" t="s">
-        <v>15</v>
+        <v>139</v>
       </c>
       <c r="E2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" t="s">
         <v>139</v>
-      </c>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" t="s">
-        <v>139</v>
-      </c>
-      <c r="B4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" t="s">
-        <v>139</v>
-      </c>
-      <c r="B5" t="s">
-        <v>60</v>
-      </c>
-      <c r="C5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E5" t="s">
-        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -1675,82 +1614,40 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="A2" sqref="A2:D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B1" t="s">
         <v>135</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>137</v>
       </c>
-      <c r="C1" t="s">
-        <v>140</v>
-      </c>
       <c r="D1" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>139</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C2">
-        <v>1965</v>
-      </c>
-      <c r="D2">
-        <v>2013</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" t="s">
+      <c r="B2" t="s">
         <v>139</v>
       </c>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3">
-        <v>1965</v>
-      </c>
-      <c r="D3">
-        <v>2013</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" t="s">
+      <c r="C2" t="s">
         <v>139</v>
       </c>
-      <c r="B4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4">
-        <v>1965</v>
-      </c>
-      <c r="D4">
-        <v>2013</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" t="s">
+      <c r="D2" t="s">
         <v>139</v>
-      </c>
-      <c r="B5" t="s">
-        <v>60</v>
-      </c>
-      <c r="C5">
-        <v>1965</v>
-      </c>
-      <c r="D5">
-        <v>2013</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add CO2 files and codes
</commit_message>
<xml_diff>
--- a/input/mappings/scaling/UNFCCC_scaling_mapping.xlsx
+++ b/input/mappings/scaling/UNFCCC_scaling_mapping.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26929"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="17280" yWindow="4820" windowWidth="25360" windowHeight="14640" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="2240" yWindow="0" windowWidth="25600" windowHeight="13940" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="map" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="201">
   <si>
     <t>description</t>
   </si>
@@ -615,6 +615,15 @@
   </si>
   <si>
     <t>1A3dii_Domestic-navigation</t>
+  </si>
+  <si>
+    <t>6.C.2</t>
+  </si>
+  <si>
+    <t>Waste-incineration</t>
+  </si>
+  <si>
+    <t>Waste incineration - Other (non-biogenic)</t>
   </si>
 </sst>
 </file>
@@ -1476,11 +1485,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E122"/>
+  <dimension ref="A1:E123"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="D28" sqref="D28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A54" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="B74" sqref="B74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2162,64 +2171,70 @@
     </row>
     <row r="73" spans="1:4">
       <c r="A73" t="s">
-        <v>91</v>
+        <v>198</v>
       </c>
       <c r="B73" t="s">
-        <v>90</v>
+        <v>200</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="D73" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="74" spans="1:4">
       <c r="A74" t="s">
-        <v>92</v>
+        <v>91</v>
+      </c>
+      <c r="B74" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="75" spans="1:4">
       <c r="A75" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="76" spans="1:4">
       <c r="A76" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="77" spans="1:4">
       <c r="A77" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="78" spans="1:4">
       <c r="A78" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4">
+      <c r="A79" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="80" spans="1:4">
-      <c r="D80" t="s">
+    <row r="81" spans="3:4">
+      <c r="D81" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="83" spans="3:4">
-      <c r="D83" s="1" t="s">
+    <row r="84" spans="3:4">
+      <c r="D84" s="1" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="84" spans="3:4">
-      <c r="D84" s="1"/>
-    </row>
     <row r="85" spans="3:4">
-      <c r="C85" t="s">
-        <v>161</v>
-      </c>
-      <c r="D85" t="s">
-        <v>112</v>
-      </c>
+      <c r="D85" s="1"/>
     </row>
     <row r="86" spans="3:4">
       <c r="C86" t="s">
         <v>161</v>
       </c>
       <c r="D86" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="87" spans="3:4">
@@ -2227,7 +2242,7 @@
         <v>161</v>
       </c>
       <c r="D87" t="s">
-        <v>132</v>
+        <v>113</v>
       </c>
     </row>
     <row r="88" spans="3:4">
@@ -2235,7 +2250,7 @@
         <v>161</v>
       </c>
       <c r="D88" t="s">
-        <v>104</v>
+        <v>132</v>
       </c>
     </row>
     <row r="89" spans="3:4">
@@ -2243,7 +2258,7 @@
         <v>161</v>
       </c>
       <c r="D89" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
     </row>
     <row r="90" spans="3:4">
@@ -2251,7 +2266,7 @@
         <v>161</v>
       </c>
       <c r="D90" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="91" spans="3:4">
@@ -2259,7 +2274,7 @@
         <v>161</v>
       </c>
       <c r="D91" t="s">
-        <v>133</v>
+        <v>115</v>
       </c>
     </row>
     <row r="92" spans="3:4">
@@ -2267,7 +2282,7 @@
         <v>161</v>
       </c>
       <c r="D92" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="93" spans="3:4">
@@ -2275,7 +2290,7 @@
         <v>161</v>
       </c>
       <c r="D93" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="94" spans="3:4">
@@ -2283,7 +2298,7 @@
         <v>161</v>
       </c>
       <c r="D94" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="95" spans="3:4">
@@ -2291,7 +2306,7 @@
         <v>161</v>
       </c>
       <c r="D95" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="96" spans="3:4">
@@ -2299,7 +2314,7 @@
         <v>161</v>
       </c>
       <c r="D96" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="97" spans="3:4">
@@ -2307,75 +2322,75 @@
         <v>161</v>
       </c>
       <c r="D97" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="98" spans="3:4">
+      <c r="C98" t="s">
+        <v>161</v>
+      </c>
+      <c r="D98" t="s">
         <v>139</v>
-      </c>
-    </row>
-    <row r="99" spans="3:4">
-      <c r="D99" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="100" spans="3:4">
       <c r="D100" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="101" spans="3:4">
       <c r="D101" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="102" spans="3:4">
       <c r="D102" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="103" spans="3:4">
       <c r="D103" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="104" spans="3:4">
+      <c r="D104" t="s">
         <v>147</v>
-      </c>
-    </row>
-    <row r="105" spans="3:4">
-      <c r="D105" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="106" spans="3:4">
       <c r="D106" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="107" spans="3:4">
       <c r="D107" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="108" spans="3:4">
       <c r="D108" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="109" spans="3:4">
+      <c r="D109" t="s">
         <v>152</v>
-      </c>
-    </row>
-    <row r="110" spans="3:4">
-      <c r="D110" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="111" spans="3:4">
       <c r="D111" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="112" spans="3:4">
+      <c r="D112" t="s">
         <v>155</v>
-      </c>
-    </row>
-    <row r="119" spans="4:5">
-      <c r="D119" t="s">
-        <v>148</v>
-      </c>
-      <c r="E119" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="120" spans="4:5">
       <c r="D120" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="E120" t="s">
         <v>164</v>
@@ -2383,7 +2398,7 @@
     </row>
     <row r="121" spans="4:5">
       <c r="D121" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E121" t="s">
         <v>164</v>
@@ -2391,15 +2406,22 @@
     </row>
     <row r="122" spans="4:5">
       <c r="D122" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E122" t="s">
         <v>164</v>
       </c>
     </row>
+    <row r="123" spans="4:5">
+      <c r="D123" t="s">
+        <v>158</v>
+      </c>
+      <c r="E123" t="s">
+        <v>164</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -2459,7 +2481,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -2472,7 +2493,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
@@ -2549,7 +2570,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>